<commit_message>
Added Matlab code etc, might work might not who knows...
</commit_message>
<xml_diff>
--- a/Stimuli/Questions.xlsx
+++ b/Stimuli/Questions.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Calvin\Desktop\SocioSpatial\SocioSpacial\Stimuli\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FED30B38-0285-4C79-83B9-FB1E52F7E026}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -475,7 +469,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -587,7 +581,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -639,7 +633,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -833,18 +827,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>